<commit_message>
preparation for v1.0.0 release
</commit_message>
<xml_diff>
--- a/input/indicators/PNC DAK_indicators.xlsx
+++ b/input/indicators/PNC DAK_indicators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/DigitalAcceleratorKits/Shared Documents/PNC DAK/_FINAL implementation tools/v0.9.9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{FC8399EC-AA32-44D8-B31A-9575EF62D96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B0C2C0C-57EE-4215-A9FC-1BE65CD8CC61}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{FC8399EC-AA32-44D8-B31A-9575EF62D96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE6DDA01-C99D-46F1-BB61-E246DD36D723}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="20" r:id="rId1"/>
@@ -123,7 +123,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
   <si>
     <r>
       <t>Digital adaptation kit for</t>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>If there are any national or global guidelines (e.g. WHO guidelines) that dictate how and why this indicator should be calculated or reported, they should be noted here. If any guidelines or recommendations change, having a clear reference listed will help in updating or restructuring your data.</t>
-  </si>
-  <si>
-    <t>https://smart.who.int/dak-pnc/v0.9.9/PNC DAK_indicators.xlsx</t>
   </si>
   <si>
     <t>© World Health Organization 2025. Some rights reserved.</t>
@@ -891,6 +888,36 @@
       <t>).</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Please access the main </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>Digital adaptation kit for postnatal care</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> document here:</t>
+    </r>
+  </si>
+  <si>
+    <t>https://iris.who.int/handle/10665/381725</t>
+  </si>
+  <si>
+    <t>https://smart.who.int/dak-pnc/v1.0.0/PNC DAK_indicators.xlsx</t>
+  </si>
 </sst>
 </file>
 
@@ -899,7 +926,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1165,10 +1192,38 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1441,7 +1496,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1541,19 +1596,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="41" fillId="4" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="43" fillId="4" borderId="5" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1583,22 +1653,19 @@
     <xf numFmtId="0" fontId="17" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="1" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1631,13 +1698,13 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="7" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="7" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="15" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="15" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="16" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="44" fillId="4" borderId="16" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5799,9 +5866,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5839,7 +5906,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5945,7 +6012,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6087,7 +6154,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6098,188 +6165,164 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:J30"/>
+  <dimension ref="A2:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D17"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="19" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="19"/>
+    <col min="1" max="1" width="4.7265625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.453125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="38.7265625" style="19" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="19"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" s="1" customFormat="1" ht="89.45" customHeight="1">
+    <row r="2" spans="2:4" s="1" customFormat="1" ht="89.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="34" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="2:4" s="1" customFormat="1" ht="15">
+    <row r="3" spans="2:4" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="2:4" s="18" customFormat="1" ht="55.5" customHeight="1">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="2:4" s="18" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
     </row>
-    <row r="5" spans="2:4" s="1" customFormat="1" ht="15.75" thickBot="1">
+    <row r="5" spans="2:4" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
     </row>
-    <row r="6" spans="2:4" s="1" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="6" spans="2:4" s="1" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="37"/>
+      <c r="D6" s="56"/>
     </row>
-    <row r="7" spans="2:4" s="21" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="7" spans="2:4" s="21" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="54"/>
     </row>
-    <row r="8" spans="2:4" s="21" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
+    <row r="8" spans="2:4" s="21" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="54"/>
     </row>
-    <row r="9" spans="2:4" s="21" customFormat="1" ht="18.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="9" spans="2:4" s="21" customFormat="1" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="54"/>
     </row>
-    <row r="10" spans="2:4" s="21" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
+    <row r="10" spans="2:4" s="21" customFormat="1" ht="17.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="54"/>
     </row>
-    <row r="11" spans="2:4" s="21" customFormat="1" ht="33.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="11" spans="2:4" s="21" customFormat="1" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="39" t="s">
+      <c r="C11" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="58"/>
     </row>
-    <row r="12" spans="2:4" s="21" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
+    <row r="12" spans="2:4" s="21" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="35"/>
+      <c r="D12" s="54"/>
     </row>
-    <row r="13" spans="2:4" s="21" customFormat="1" ht="35.25" customHeight="1" thickTop="1" thickBot="1">
+    <row r="13" spans="2:4" s="21" customFormat="1" ht="35.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="38"/>
+      <c r="D13" s="57"/>
     </row>
-    <row r="14" spans="2:4" s="21" customFormat="1" ht="15.4" customHeight="1" thickTop="1" thickBot="1">
+    <row r="14" spans="2:4" s="21" customFormat="1" ht="15.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="38"/>
+      <c r="D14" s="57"/>
     </row>
-    <row r="15" spans="2:4" s="21" customFormat="1" ht="46.9" customHeight="1" thickTop="1" thickBot="1">
+    <row r="15" spans="2:4" s="21" customFormat="1" ht="46.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="38"/>
+      <c r="D15" s="57"/>
     </row>
-    <row r="16" spans="2:4" s="21" customFormat="1" ht="15.75" thickTop="1"/>
-    <row r="17" spans="2:10" s="21" customFormat="1" ht="15">
-      <c r="B17" s="65" t="s">
+    <row r="16" spans="2:4" s="21" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:10" s="25" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="35"/>
+      <c r="B17" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+    </row>
+    <row r="18" spans="1:10" s="21" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:10" s="21" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="20" spans="1:10" s="21" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="70"/>
+      <c r="D20" s="71"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="66"/>
-      <c r="D17" s="67"/>
-    </row>
-    <row r="18" spans="2:10" ht="12.75" customHeight="1">
-      <c r="B18" s="49" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="50"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-    </row>
-    <row r="19" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B19" s="49" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-    </row>
-    <row r="20" spans="2:10" ht="42" customHeight="1">
-      <c r="B20" s="49" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-    </row>
-    <row r="21" spans="2:10" ht="27.75" customHeight="1">
-      <c r="B21" s="52" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="53"/>
-      <c r="D21" s="54"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
       <c r="G21" s="21"/>
@@ -6287,12 +6330,12 @@
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
     </row>
-    <row r="22" spans="2:10" ht="48" customHeight="1">
-      <c r="B22" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="44"/>
-      <c r="D22" s="45"/>
+    <row r="22" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41"/>
       <c r="E22" s="21"/>
       <c r="F22" s="21"/>
       <c r="G22" s="21"/>
@@ -6300,12 +6343,12 @@
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
     </row>
-    <row r="23" spans="2:10" ht="28.5" customHeight="1">
-      <c r="B23" s="43" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="45"/>
+    <row r="23" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
       <c r="G23" s="21"/>
@@ -6313,12 +6356,12 @@
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="2:10" ht="26.25" customHeight="1">
-      <c r="B24" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45"/>
+    <row r="24" spans="1:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="21"/>
       <c r="F24" s="21"/>
       <c r="G24" s="21"/>
@@ -6326,12 +6369,12 @@
       <c r="I24" s="21"/>
       <c r="J24" s="21"/>
     </row>
-    <row r="25" spans="2:10" ht="21" customHeight="1">
-      <c r="B25" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="44"/>
-      <c r="D25" s="45"/>
+    <row r="25" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
@@ -6339,12 +6382,12 @@
       <c r="I25" s="21"/>
       <c r="J25" s="21"/>
     </row>
-    <row r="26" spans="2:10" ht="42" customHeight="1">
-      <c r="B26" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
+    <row r="26" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="21"/>
       <c r="F26" s="21"/>
       <c r="G26" s="21"/>
@@ -6352,12 +6395,12 @@
       <c r="I26" s="21"/>
       <c r="J26" s="21"/>
     </row>
-    <row r="27" spans="2:10" ht="47.25" customHeight="1">
-      <c r="B27" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="42"/>
+    <row r="27" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
       <c r="G27" s="21"/>
@@ -6365,12 +6408,12 @@
       <c r="I27" s="21"/>
       <c r="J27" s="21"/>
     </row>
-    <row r="28" spans="2:10" ht="39" customHeight="1">
-      <c r="B28" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="45"/>
+    <row r="28" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
       <c r="E28" s="21"/>
       <c r="F28" s="21"/>
       <c r="G28" s="21"/>
@@ -6378,12 +6421,12 @@
       <c r="I28" s="21"/>
       <c r="J28" s="21"/>
     </row>
-    <row r="29" spans="2:10" ht="41.25" customHeight="1">
-      <c r="B29" s="46" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="47"/>
-      <c r="D29" s="48"/>
+    <row r="29" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="46"/>
+      <c r="D29" s="47"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21"/>
       <c r="G29" s="21"/>
@@ -6391,7 +6434,12 @@
       <c r="I29" s="21"/>
       <c r="J29" s="21"/>
     </row>
-    <row r="30" spans="2:10" ht="15">
+    <row r="30" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="46"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="21"/>
       <c r="F30" s="21"/>
       <c r="G30" s="21"/>
@@ -6399,21 +6447,43 @@
       <c r="I30" s="21"/>
       <c r="J30" s="21"/>
     </row>
+    <row r="31" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="49"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+    </row>
+    <row r="32" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="52"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+    </row>
+    <row r="33" spans="5:10" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+    </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
     <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B17:D17"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="C6:D6"/>
@@ -6425,14 +6495,27 @@
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B29:D29"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B17" r:id="rId1" xr:uid="{B0B72D77-0D0D-4D71-B386-72B5E9B8B90C}"/>
-    <hyperlink ref="B17:D17" r:id="rId2" display="https://smart.who.int/dak-pnc/v0.9.9/PNC DAK_indicators.xlsx" xr:uid="{4CC2310C-BE7E-4EE3-9A68-9B26A7CF4C01}"/>
+    <hyperlink ref="B20" r:id="rId1" xr:uid="{B0B72D77-0D0D-4D71-B386-72B5E9B8B90C}"/>
+    <hyperlink ref="B20:D20" r:id="rId2" display="https://smart.who.int/dak-pnc/v0.9.9/PNC DAK_indicators.xlsx" xr:uid="{4CC2310C-BE7E-4EE3-9A68-9B26A7CF4C01}"/>
+    <hyperlink ref="C17" r:id="rId3" xr:uid="{7CF94869-48E0-4734-A70D-A822869CF9EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -6445,22 +6528,22 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" style="25" customWidth="1"/>
     <col min="2" max="2" width="18" style="25" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" style="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" style="25" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" style="25" customWidth="1"/>
+    <col min="5" max="5" width="30.453125" style="25" customWidth="1"/>
     <col min="6" max="6" width="20" style="25" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" style="25" customWidth="1"/>
-    <col min="9" max="9" width="56.42578125" style="25" customWidth="1"/>
-    <col min="10" max="10" width="37.7109375" style="25" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="25"/>
+    <col min="7" max="7" width="24.7265625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="27.453125" style="25" customWidth="1"/>
+    <col min="9" max="9" width="56.453125" style="25" customWidth="1"/>
+    <col min="10" max="10" width="37.7265625" style="25" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" s="18" customFormat="1" ht="15">
+    <row r="1" spans="2:16" s="18" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="B1" s="23"/>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -6470,29 +6553,29 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="2:16" ht="15">
-      <c r="B2" s="60" t="s">
+    <row r="2" spans="2:16" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B2" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="D2" s="60" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="10"/>
+      <c r="I2" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="62" t="s">
         <v>37</v>
-      </c>
-      <c r="H2" s="10"/>
-      <c r="I2" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>38</v>
       </c>
       <c r="K2" s="24"/>
       <c r="L2" s="24"/>
@@ -6501,24 +6584,24 @@
       <c r="O2" s="24"/>
       <c r="P2" s="24"/>
     </row>
-    <row r="3" spans="2:16" ht="15">
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="57"/>
+    <row r="3" spans="2:16" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="61"/>
       <c r="E3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>40</v>
-      </c>
       <c r="G3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="57"/>
-      <c r="J3" s="59"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="63"/>
       <c r="K3" s="24"/>
       <c r="L3" s="24"/>
       <c r="M3" s="24"/>
@@ -6526,218 +6609,218 @@
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
     </row>
-    <row r="4" spans="2:16" s="2" customFormat="1" ht="15">
-      <c r="B4" s="62" t="s">
+    <row r="4" spans="2:16" s="2" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B4" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
+    </row>
+    <row r="5" spans="2:16" ht="83.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="64"/>
+      <c r="C5" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" spans="2:16" ht="83.65" customHeight="1">
-      <c r="B5" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="28" t="s">
+    <row r="6" spans="2:16" ht="89" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="119.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="30" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="72.5" x14ac:dyDescent="0.25">
+      <c r="B8" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="29" t="s">
+      <c r="I8" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="15" t="s">
-        <v>50</v>
-      </c>
     </row>
-    <row r="6" spans="2:16" ht="92.25">
-      <c r="B6" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="E6" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="29" t="s">
+    <row r="9" spans="2:16" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="66" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="67"/>
+      <c r="H9" s="67"/>
+      <c r="I9" s="67"/>
+      <c r="J9" s="68"/>
+    </row>
+    <row r="10" spans="2:16" s="26" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="30" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="H11" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>50</v>
+      <c r="I11" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="J11" s="33" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="119.65" customHeight="1">
-      <c r="B7" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" ht="90">
-      <c r="B8" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="15">
-      <c r="B9" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="63"/>
-      <c r="J9" s="64"/>
-    </row>
-    <row r="10" spans="2:16" s="26" customFormat="1" ht="79.5" customHeight="1">
-      <c r="B10" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="J10" s="32" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="96.75" customHeight="1">
-      <c r="B11" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="J11" s="33" t="s">
+    <row r="12" spans="2:16" ht="33.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="59" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" ht="33.4" customHeight="1">
-      <c r="B12" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="55"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="55"/>
-      <c r="G12" s="55"/>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="55"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -6764,65 +6847,65 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="78.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="5"/>
+    <col min="1" max="1" width="4.1796875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="78.7265625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="61.7265625" style="5" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.25" customHeight="1">
+    <row r="2" spans="1:3" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>91</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" ht="45">
+    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>93</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" ht="45.4" customHeight="1">
+    <row r="4" spans="1:3" ht="45.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45">
+    <row r="5" spans="1:3" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="16"/>
     </row>
   </sheetData>
@@ -6832,103 +6915,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
-      <UserInfo>
-        <DisplayName>NASH-MENDEZ, Natschja</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Pete Christopher (Green Ink) (p.christopher@greenink.co.uk)</DisplayName>
-        <AccountId>26</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
-        <AccountId>13</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>AMIN, Avni</DisplayName>
-        <AccountId>46</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>GARCIA MORENO ESTEVA, Claudia M.</DisplayName>
-        <AccountId>47</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
-        <AccountId>61</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TITI-OFEI, Regina</DisplayName>
-        <AccountId>62</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>COSMAS, Leonard</DisplayName>
-        <AccountId>63</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>BONET SEMENAS, Mercedes</DisplayName>
-        <AccountId>94</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>PORTELA, Anayda Gerarda</DisplayName>
-        <AccountId>302</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>samira.m.haddad</DisplayName>
-        <AccountId>284</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>CONWAY, Francesca</DisplayName>
-        <AccountId>283</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TUNCALP, Özge</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>TAMRAT, Tigest</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="73389989-ac93-4f39-a9f3-2949bbf25fcc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A6DDC313EDC9A43B330D8B6305883A5" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5b0342cd22268e5e5d3683a3cff816e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73389989-ac93-4f39-a9f3-2949bbf25fcc" xmlns:ns3="51983ca6-de84-41fa-9a65-1d08ee1009bc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c638d06e48d95e9efa3bb75773f50cd7" ns2:_="" ns3:_="">
     <xsd:import namespace="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
@@ -7183,14 +7169,143 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc">
+      <UserInfo>
+        <DisplayName>NASH-MENDEZ, Natschja</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Pete Christopher (Green Ink) (p.christopher@greenink.co.uk)</DisplayName>
+        <AccountId>26</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BARREIX ETCHEGOIMBERRY, Maria</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>AMIN, Avni</DisplayName>
+        <AccountId>46</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>GARCIA MORENO ESTEVA, Claudia M.</DisplayName>
+        <AccountId>47</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>KIPRUTO, Hillary Kipchumba</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>SEYDI, Aminata Binetou Wahebine</DisplayName>
+        <AccountId>61</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TITI-OFEI, Regina</DisplayName>
+        <AccountId>62</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>COSMAS, Leonard</DisplayName>
+        <AccountId>63</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>BONET SEMENAS, Mercedes</DisplayName>
+        <AccountId>94</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>PORTELA, Anayda Gerarda</DisplayName>
+        <AccountId>302</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>samira.m.haddad</DisplayName>
+        <AccountId>284</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>CONWAY, Francesca</DisplayName>
+        <AccountId>283</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TUNCALP, Özge</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>TAMRAT, Tigest</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="73389989-ac93-4f39-a9f3-2949bbf25fcc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{924A4ACD-5488-46C8-ABF3-D5050B19848E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{924A4ACD-5488-46C8-ABF3-D5050B19848E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>